<commit_message>
added CoolMasterNet log handling, better error handling for missing mapped indexes
</commit_message>
<xml_diff>
--- a/Projects/McGuigan/Mapping Data/RTI Diagnostics Feed Info - McGuigan.xlsx
+++ b/Projects/McGuigan/Mapping Data/RTI Diagnostics Feed Info - McGuigan.xlsx
@@ -8,11 +8,10 @@
     <sheet state="visible" name="Source List" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Audio Zones" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="Video Zones" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="RCM12 List" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="Ports List" sheetId="6" r:id="rId9"/>
     <sheet state="visible" name="Lighting Loads" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="Lighting Keypads" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="Task List" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="Button List" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="Task List" sheetId="8" r:id="rId11"/>
+    <sheet state="visible" name="Button List" sheetId="9" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="332">
   <si>
     <t>Room Index</t>
   </si>
@@ -493,556 +492,529 @@
     <t>Suite Bath Fan</t>
   </si>
   <si>
+    <t>Task Index</t>
+  </si>
+  <si>
+    <t>Task Name</t>
+  </si>
+  <si>
+    <t>East Bed Bath Fan 5 min - TOGGLE</t>
+  </si>
+  <si>
+    <t>Test - Family LED On Scene with Raise</t>
+  </si>
+  <si>
+    <t>Test - Family LED Off with Lower</t>
+  </si>
+  <si>
+    <t>Test - Family LED On Full with Raise</t>
+  </si>
+  <si>
+    <t>Test - Family LED On Dim with Raise</t>
+  </si>
+  <si>
+    <t>Audio - Zone 1 Power On</t>
+  </si>
+  <si>
+    <t>Audio - Zone 1 Power Off</t>
+  </si>
+  <si>
+    <t>Audio - Zone 1 Mute On</t>
+  </si>
+  <si>
+    <t>Audio - Zone 1 Mute Off</t>
+  </si>
+  <si>
+    <t>Audio - Zone 1 Vol + Press vs Hold Logic</t>
+  </si>
+  <si>
+    <t>Audio - Zone 1 Vol +</t>
+  </si>
+  <si>
+    <t>Audio - Zone 1 Vol -</t>
+  </si>
+  <si>
+    <t>Audio - Zone 1 Vol - Press vs Hold Logic</t>
+  </si>
+  <si>
+    <t>Construction On with Raise</t>
+  </si>
+  <si>
+    <t>Construction Off with Lower</t>
+  </si>
+  <si>
+    <t>Bottom Floor Laundry Room /Fan 30 min - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Bottom Floor Hallway - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Wine Room Shelf and A - Toggle Dim</t>
+  </si>
+  <si>
+    <t>Billiards Area - GAMING SCENE - Toggle</t>
+  </si>
+  <si>
+    <t>Billiards Area - ROOM OFF</t>
+  </si>
+  <si>
+    <t>Suite Bath - ROOM OFF</t>
+  </si>
+  <si>
+    <t>East Bed Bath - ROOM OFF</t>
+  </si>
+  <si>
+    <t>Powder Room - ROOM OFF</t>
+  </si>
+  <si>
+    <t>Office - ROOM OFF</t>
+  </si>
+  <si>
+    <t>Living Room - ROOM OFF</t>
+  </si>
+  <si>
+    <t>Dining Room - ROOM OFF</t>
+  </si>
+  <si>
+    <t>Family Room - ROOM OFF</t>
+  </si>
+  <si>
+    <t>Kitchen - ROOM OFF</t>
+  </si>
+  <si>
+    <t>Garage - ROOM OFF</t>
+  </si>
+  <si>
+    <t>East Bed - ROOM OFF</t>
+  </si>
+  <si>
+    <t>Main Bed - ROOM OFF</t>
+  </si>
+  <si>
+    <t>Main Bed Bath - ROOM OFF</t>
+  </si>
+  <si>
+    <t>West Bed - ROOM OFF</t>
+  </si>
+  <si>
+    <t>Gym - ROOM OFF</t>
+  </si>
+  <si>
+    <t>Pool - ROOM OFF</t>
+  </si>
+  <si>
+    <t>Wine Room - ROOM OFF</t>
+  </si>
+  <si>
+    <t>Suite Kitchen - ROOM OFF</t>
+  </si>
+  <si>
+    <t>Suite Living Room - ROOM OFF</t>
+  </si>
+  <si>
+    <t>Suite Bed - ROOM OFF</t>
+  </si>
+  <si>
+    <t>Powder Room - MOTION (Day/Night)</t>
+  </si>
+  <si>
+    <t>East Bed Bath - MOTION (Day/Night)</t>
+  </si>
+  <si>
+    <t>West Bed Bath - MOTION (Day/Night)</t>
+  </si>
+  <si>
+    <t>Billiards Area Bath - MOTION (Day/Night)</t>
+  </si>
+  <si>
+    <t>Suite Bath - MOTION (Day/Night)</t>
+  </si>
+  <si>
+    <t>Main Bed Walk-In - MOTION (Day/Night)</t>
+  </si>
+  <si>
+    <t>Powder Room Hallway North Closet - DOOR CONTACTS</t>
+  </si>
+  <si>
+    <t>Billiards Area - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Gym - Dim TOGGLE</t>
+  </si>
+  <si>
+    <t>Bottom Floor Stairs - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Pool - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Billiards Area Bath - ROOM OFF</t>
+  </si>
+  <si>
+    <t>Billiards Area Bath - DAILY SCENE</t>
+  </si>
+  <si>
+    <t>Billiards Area Bath - BRIGHT SCENE</t>
+  </si>
+  <si>
+    <t>Pool Patio - SWITCH TOGGLE</t>
+  </si>
+  <si>
+    <t>Gym Patio - SWITCH TOGGLE</t>
+  </si>
+  <si>
+    <t>Sauna - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Storage Room Under Garage - SWITCH TOGGLE</t>
+  </si>
+  <si>
+    <t>Front Exterior Micro Recessed - SWITCH TOGGLE</t>
+  </si>
+  <si>
+    <t>Bottom Floor Mech Room - SWITCH TOGGLE</t>
+  </si>
+  <si>
+    <t>Bottom Floor Laundry Fan 30 min - TOGGLE</t>
+  </si>
+  <si>
+    <t>Billiards Area Bath Fan 30 min - TOGGLE</t>
+  </si>
+  <si>
+    <t>Suite Bath - DAILY SCENE</t>
+  </si>
+  <si>
+    <t>Suite Bath - BRIGHT SCENE</t>
+  </si>
+  <si>
+    <t>East Bed Bath - DAILY SCENE</t>
+  </si>
+  <si>
+    <t>East Bed Bath - BRIGHT SCENE</t>
+  </si>
+  <si>
+    <t>West Bed Bath - ROOM OFF</t>
+  </si>
+  <si>
+    <t>West Bed Bath - BRIGHT SCENE</t>
+  </si>
+  <si>
+    <t>West Bed Bath - DAILY SCENE</t>
+  </si>
+  <si>
+    <t>West Bed - BRIGHT SCENE</t>
+  </si>
+  <si>
+    <t>West Bed - DAILY SCENE</t>
+  </si>
+  <si>
+    <t>Powder Room - BRIGHT SCENE</t>
+  </si>
+  <si>
+    <t>Powder Room - DAILY SCENE</t>
+  </si>
+  <si>
+    <t>Powder Room Fan 30 min - TOGGLE</t>
+  </si>
+  <si>
+    <t>Main Bed - DAILY SCENE</t>
+  </si>
+  <si>
+    <t>Main Bed Sitting Area - DIM</t>
+  </si>
+  <si>
+    <t>Main Bed/East Bed Patio - SWITCH TOGGLE</t>
+  </si>
+  <si>
+    <t>Main Bed Bath/West Bed Patio - SWITCH TOGGLE</t>
+  </si>
+  <si>
+    <t>Office - DAILY SCENE</t>
+  </si>
+  <si>
+    <t>Office Patio - SWITCH TOGGLE</t>
+  </si>
+  <si>
+    <t>Kitchen Patio - SWITCH TOGGLE</t>
+  </si>
+  <si>
+    <t>ALL Lower Patio - SWITCH TOGGLE</t>
+  </si>
+  <si>
+    <t>Suite Sitting Area - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Suite Kitchen Recessed - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Suite Kitchen Counter - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Suite Bed - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Suite Bath Fan 30 min - TOGGLE</t>
+  </si>
+  <si>
+    <t>Suite Fireplace 2 hr- TOGGLE</t>
+  </si>
+  <si>
+    <t>Entrance/Dining Fireplace 2 hr- TOGGLE</t>
+  </si>
+  <si>
+    <t>Main Bed Fireplace 2 hr- TOGGLE</t>
+  </si>
+  <si>
+    <t>Pool Fireplace 2 hr- TOGGLE</t>
+  </si>
+  <si>
+    <t>East Bed Closet - MOTION (Day/Night)</t>
+  </si>
+  <si>
+    <t>West Bed Closet - MOTION (Day/Night)</t>
+  </si>
+  <si>
+    <t>Powder Room Hallway South Closet - DOOR CONTACTS</t>
+  </si>
+  <si>
+    <t>Suite Bed Closet - DOOR CONTACTS</t>
+  </si>
+  <si>
+    <t>Kitchen - DAILY SCENE</t>
+  </si>
+  <si>
+    <t>Kitchen/Family - DIM SCENE</t>
+  </si>
+  <si>
+    <t>Family Room - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Dining Patio - SWITCH TOGGLE</t>
+  </si>
+  <si>
+    <t>Dining Room - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Dining Room Table - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Top Floor Stairs - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Middle Floor Hallway - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Top Floor Hallway - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Middle Floor Laundry Room/Fan 30 min - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Main Electrical Room - SWITCH TOGGLE</t>
+  </si>
+  <si>
+    <t>East Bed - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>East Bed Closet - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>West Bed Closet - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>West Bed Bath Fan 30 min - TOGGLE</t>
+  </si>
+  <si>
+    <t>Main Bed Walk-In - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Main Bed Bath - MOTION (Day/Night)</t>
+  </si>
+  <si>
+    <t>Main Bed Bath - DAILY SCENE</t>
+  </si>
+  <si>
+    <t>Main Bed Bath - BRIGHT SCENE</t>
+  </si>
+  <si>
+    <t>Main Bed Bath - NIGHT SCENE</t>
+  </si>
+  <si>
+    <t>Main Bed Bath Shower - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Main Bed Bath Fan 30 min - TOGGLE</t>
+  </si>
+  <si>
+    <t>Wine Room Closet - SWITCH TOGGLE</t>
+  </si>
+  <si>
+    <t>Suite Kitchen - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Living Room - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Garage Lights - SWITCH TOGGLE</t>
+  </si>
+  <si>
+    <t>Main Bed East Closet - MOTION (Day/Night)</t>
+  </si>
+  <si>
+    <t>Suite Bed Closet - MOTION (Day/Night)</t>
+  </si>
+  <si>
+    <t>East Bed Bath Shower - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Pantry - DIM TOGGLE</t>
+  </si>
+  <si>
+    <t>Wine Room - MOTION</t>
+  </si>
+  <si>
+    <t>Lower Hall - MOTION</t>
+  </si>
+  <si>
+    <t>Art Scene - UNKNOWN - Toggle</t>
+  </si>
+  <si>
+    <t>Bottom Floor Stairs - SWITCH ON</t>
+  </si>
+  <si>
+    <t>Pool Colored Lights - SWITCH TOGGLE</t>
+  </si>
+  <si>
+    <t>Jacuzzi Heater - TOGGLE LED FOR RTI</t>
+  </si>
+  <si>
+    <t>Jacuzzi Heater v2 - TOGGLE TASK LEDS</t>
+  </si>
+  <si>
+    <t>Whole House - GUEST SCENE</t>
+  </si>
+  <si>
+    <t>Whole House - OUTDOOR SCENE</t>
+  </si>
+  <si>
+    <t>Whole House - HOUSE OFF</t>
+  </si>
+  <si>
+    <t>Whole House - GOODBYE SCENE</t>
+  </si>
+  <si>
+    <t>Whole House - SLEEP SCENE</t>
+  </si>
+  <si>
+    <t>Whole House - MORNING SCENE</t>
+  </si>
+  <si>
+    <t>Whole House - BACKYARD SCENE TOGGLE</t>
+  </si>
+  <si>
+    <t>Jacuzzi Heater ON</t>
+  </si>
+  <si>
+    <t>Jacuzzi Heater OFF</t>
+  </si>
+  <si>
+    <t>Jacuzzi Heater v2 - TASK LED ON</t>
+  </si>
+  <si>
+    <t>Jacuzzi Heater v2 - TASK LED OFF</t>
+  </si>
+  <si>
+    <t>Volume + POOL ROOM</t>
+  </si>
+  <si>
+    <t>Volume - POOL ROOM</t>
+  </si>
+  <si>
+    <t>Gym - Exercise TOGGLE</t>
+  </si>
+  <si>
+    <t>Valence Lights ALL - Toggle</t>
+  </si>
+  <si>
+    <t>Volume + BILLIARDS AREA</t>
+  </si>
+  <si>
+    <t>Volume - BILLIARDS AREA</t>
+  </si>
+  <si>
+    <t>Volume + SUITE KITCHEN</t>
+  </si>
+  <si>
+    <t>Volume - SUITE KITCHEN</t>
+  </si>
+  <si>
+    <t>Volume + MAIN BED BATH</t>
+  </si>
+  <si>
+    <t>Volume - MAIN BED BATH</t>
+  </si>
+  <si>
+    <t>Volume + DINING ROOM</t>
+  </si>
+  <si>
+    <t>Volume - DINING ROOM</t>
+  </si>
+  <si>
+    <t>Whole House -BRIGHT SCENE</t>
+  </si>
+  <si>
+    <t>Whole House -RELAX SCENE</t>
+  </si>
+  <si>
+    <t>Pool Camera Shut Off 3 hrs</t>
+  </si>
+  <si>
+    <t>East Bed Bath - OCC (Day/Night)</t>
+  </si>
+  <si>
+    <t>West Bed Bath - OCC (Day/Night)</t>
+  </si>
+  <si>
+    <t>Suite Bath - OCC (Day/Night)</t>
+  </si>
+  <si>
+    <t>Main Bed Bath - OCC (Day/Night)</t>
+  </si>
+  <si>
+    <t>Powder Room - OCC (Day/Night)</t>
+  </si>
+  <si>
+    <t>Billiards Area Bath - OCC (Day/Night)</t>
+  </si>
+  <si>
+    <t>East Bed Closet - OCC (Day/Night)</t>
+  </si>
+  <si>
+    <t>Main Bed Walk-In - OCC (Day/Night)</t>
+  </si>
+  <si>
+    <t>West Bed Closet - OCC (Day/Night)</t>
+  </si>
+  <si>
+    <t>Main Bed East Closet - OCC (Day/Night)</t>
+  </si>
+  <si>
+    <t>Suite Bed Closet - OCC (Day/Night)</t>
+  </si>
+  <si>
+    <t>Wine Room - OCC</t>
+  </si>
+  <si>
+    <t>Lower Hall - OCC</t>
+  </si>
+  <si>
+    <t>East and West Patio - SWITCH TOGGLE</t>
+  </si>
+  <si>
     <t>Button Index</t>
   </si>
   <si>
     <t>Button Name</t>
-  </si>
-  <si>
-    <t>Button VID</t>
-  </si>
-  <si>
-    <t>Task Index</t>
-  </si>
-  <si>
-    <t>Task Name</t>
-  </si>
-  <si>
-    <t>East Bed Bath Fan 5 min - TOGGLE</t>
-  </si>
-  <si>
-    <t>Test - Family LED On Scene with Raise</t>
-  </si>
-  <si>
-    <t>Test - Family LED Off with Lower</t>
-  </si>
-  <si>
-    <t>Test - Family LED On Full with Raise</t>
-  </si>
-  <si>
-    <t>Test - Family LED On Dim with Raise</t>
-  </si>
-  <si>
-    <t>Audio - Zone 1 Power On</t>
-  </si>
-  <si>
-    <t>Audio - Zone 1 Power Off</t>
-  </si>
-  <si>
-    <t>Audio - Zone 1 Mute On</t>
-  </si>
-  <si>
-    <t>Audio - Zone 1 Mute Off</t>
-  </si>
-  <si>
-    <t>Audio - Zone 1 Vol + Press vs Hold Logic</t>
-  </si>
-  <si>
-    <t>Audio - Zone 1 Vol +</t>
-  </si>
-  <si>
-    <t>Audio - Zone 1 Vol -</t>
-  </si>
-  <si>
-    <t>Audio - Zone 1 Vol - Press vs Hold Logic</t>
-  </si>
-  <si>
-    <t>Construction On with Raise</t>
-  </si>
-  <si>
-    <t>Construction Off with Lower</t>
-  </si>
-  <si>
-    <t>Bottom Floor Laundry Room /Fan 30 min - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Bottom Floor Hallway - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Wine Room Shelf and A - Toggle Dim</t>
-  </si>
-  <si>
-    <t>Billiards Area - GAMING SCENE - Toggle</t>
-  </si>
-  <si>
-    <t>Billiards Area - ROOM OFF</t>
-  </si>
-  <si>
-    <t>Suite Bath - ROOM OFF</t>
-  </si>
-  <si>
-    <t>East Bed Bath - ROOM OFF</t>
-  </si>
-  <si>
-    <t>Powder Room - ROOM OFF</t>
-  </si>
-  <si>
-    <t>Office - ROOM OFF</t>
-  </si>
-  <si>
-    <t>Living Room - ROOM OFF</t>
-  </si>
-  <si>
-    <t>Dining Room - ROOM OFF</t>
-  </si>
-  <si>
-    <t>Family Room - ROOM OFF</t>
-  </si>
-  <si>
-    <t>Kitchen - ROOM OFF</t>
-  </si>
-  <si>
-    <t>Garage - ROOM OFF</t>
-  </si>
-  <si>
-    <t>East Bed - ROOM OFF</t>
-  </si>
-  <si>
-    <t>Main Bed - ROOM OFF</t>
-  </si>
-  <si>
-    <t>Main Bed Bath - ROOM OFF</t>
-  </si>
-  <si>
-    <t>West Bed - ROOM OFF</t>
-  </si>
-  <si>
-    <t>Gym - ROOM OFF</t>
-  </si>
-  <si>
-    <t>Pool - ROOM OFF</t>
-  </si>
-  <si>
-    <t>Wine Room - ROOM OFF</t>
-  </si>
-  <si>
-    <t>Vantage Controls</t>
-  </si>
-  <si>
-    <t>Inc.</t>
-  </si>
-  <si>
-    <t>Page 1 of 5</t>
-  </si>
-  <si>
-    <t>Suite Kitchen - ROOM OFF</t>
-  </si>
-  <si>
-    <t>Suite Living Room - ROOM OFF</t>
-  </si>
-  <si>
-    <t>Suite Bed - ROOM OFF</t>
-  </si>
-  <si>
-    <t>Powder Room - MOTION (Day/Night)</t>
-  </si>
-  <si>
-    <t>East Bed Bath - MOTION (Day/Night)</t>
-  </si>
-  <si>
-    <t>West Bed Bath - MOTION (Day/Night)</t>
-  </si>
-  <si>
-    <t>Billiards Area Bath - MOTION (Day/Night)</t>
-  </si>
-  <si>
-    <t>Suite Bath - MOTION (Day/Night)</t>
-  </si>
-  <si>
-    <t>Main Bed Walk-In - MOTION (Day/Night)</t>
-  </si>
-  <si>
-    <t>Powder Room Hallway North Closet - DOOR CONTACTS</t>
-  </si>
-  <si>
-    <t>Billiards Area - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Gym - Dim TOGGLE</t>
-  </si>
-  <si>
-    <t>Bottom Floor Stairs - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Pool - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Billiards Area Bath - ROOM OFF</t>
-  </si>
-  <si>
-    <t>Billiards Area Bath - DAILY SCENE</t>
-  </si>
-  <si>
-    <t>Billiards Area Bath - BRIGHT SCENE</t>
-  </si>
-  <si>
-    <t>Pool Patio - SWITCH TOGGLE</t>
-  </si>
-  <si>
-    <t>Gym Patio - SWITCH TOGGLE</t>
-  </si>
-  <si>
-    <t>Sauna - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Storage Room Under Garage - SWITCH TOGGLE</t>
-  </si>
-  <si>
-    <t>Front Exterior Micro Recessed - SWITCH TOGGLE</t>
-  </si>
-  <si>
-    <t>Bottom Floor Mech Room - SWITCH TOGGLE</t>
-  </si>
-  <si>
-    <t>Bottom Floor Laundry Fan 30 min - TOGGLE</t>
-  </si>
-  <si>
-    <t>Billiards Area Bath Fan 30 min - TOGGLE</t>
-  </si>
-  <si>
-    <t>Suite Bath - DAILY SCENE</t>
-  </si>
-  <si>
-    <t>Suite Bath - BRIGHT SCENE</t>
-  </si>
-  <si>
-    <t>East Bed Bath - DAILY SCENE</t>
-  </si>
-  <si>
-    <t>East Bed Bath - BRIGHT SCENE</t>
-  </si>
-  <si>
-    <t>West Bed Bath - ROOM OFF</t>
-  </si>
-  <si>
-    <t>West Bed Bath - BRIGHT SCENE</t>
-  </si>
-  <si>
-    <t>West Bed Bath - DAILY SCENE</t>
-  </si>
-  <si>
-    <t>West Bed - BRIGHT SCENE</t>
-  </si>
-  <si>
-    <t>West Bed - DAILY SCENE</t>
-  </si>
-  <si>
-    <t>Powder Room - BRIGHT SCENE</t>
-  </si>
-  <si>
-    <t>Powder Room - DAILY SCENE</t>
-  </si>
-  <si>
-    <t>Powder Room Fan 30 min - TOGGLE</t>
-  </si>
-  <si>
-    <t>Main Bed - DAILY SCENE</t>
-  </si>
-  <si>
-    <t>Main Bed Sitting Area - DIM</t>
-  </si>
-  <si>
-    <t>Page 2 of 5</t>
-  </si>
-  <si>
-    <t>TOGGLE</t>
-  </si>
-  <si>
-    <t>Main Bed/East Bed Patio - SWITCH TOGGLE</t>
-  </si>
-  <si>
-    <t>Main Bed Bath/West Bed Patio - SWITCH TOGGLE</t>
-  </si>
-  <si>
-    <t>Office - DAILY SCENE</t>
-  </si>
-  <si>
-    <t>Office Patio - SWITCH TOGGLE</t>
-  </si>
-  <si>
-    <t>Kitchen Patio - SWITCH TOGGLE</t>
-  </si>
-  <si>
-    <t>ALL Lower Patio - SWITCH TOGGLE</t>
-  </si>
-  <si>
-    <t>Suite Sitting Area - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Suite Kitchen Recessed - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Suite Kitchen Counter - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Suite Bed - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Suite Bath Fan 30 min - TOGGLE</t>
-  </si>
-  <si>
-    <t>Suite Fireplace 2 hr- TOGGLE</t>
-  </si>
-  <si>
-    <t>Entrance/Dining Fireplace 2 hr- TOGGLE</t>
-  </si>
-  <si>
-    <t>Main Bed Fireplace 2 hr- TOGGLE</t>
-  </si>
-  <si>
-    <t>Pool Fireplace 2 hr- TOGGLE</t>
-  </si>
-  <si>
-    <t>East Bed Closet - MOTION (Day/Night)</t>
-  </si>
-  <si>
-    <t>West Bed Closet - MOTION (Day/Night)</t>
-  </si>
-  <si>
-    <t>Powder Room Hallway South Closet - DOOR CONTACTS</t>
-  </si>
-  <si>
-    <t>Suite Bed Closet - DOOR CONTACTS</t>
-  </si>
-  <si>
-    <t>Kitchen - DAILY SCENE</t>
-  </si>
-  <si>
-    <t>Kitchen/Family - DIM SCENE</t>
-  </si>
-  <si>
-    <t>Family Room - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Dining Patio - SWITCH TOGGLE</t>
-  </si>
-  <si>
-    <t>Dining Room - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Dining Room Table - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Top Floor Stairs - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Middle Floor Hallway - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Top Floor Hallway - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Middle Floor Laundry Room/Fan 30 min - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Main Electrical Room - SWITCH TOGGLE</t>
-  </si>
-  <si>
-    <t>East Bed - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>East Bed Closet - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>West Bed Closet - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>West Bed Bath Fan 30 min - TOGGLE</t>
-  </si>
-  <si>
-    <t>Main Bed Walk-In - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Main Bed Bath - MOTION (Day/Night)</t>
-  </si>
-  <si>
-    <t>Main Bed Bath - DAILY SCENE</t>
-  </si>
-  <si>
-    <t>Page 3 of 5</t>
-  </si>
-  <si>
-    <t>Main Bed Bath - BRIGHT SCENE</t>
-  </si>
-  <si>
-    <t>Main Bed Bath - NIGHT SCENE</t>
-  </si>
-  <si>
-    <t>Main Bed Bath Shower - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Main Bed Bath Fan 30 min - TOGGLE</t>
-  </si>
-  <si>
-    <t>Wine Room Closet - SWITCH TOGGLE</t>
-  </si>
-  <si>
-    <t>Suite Kitchen - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Living Room - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Garage Lights - SWITCH TOGGLE</t>
-  </si>
-  <si>
-    <t>Main Bed East Closet - MOTION (Day/Night)</t>
-  </si>
-  <si>
-    <t>Suite Bed Closet - MOTION (Day/Night)</t>
-  </si>
-  <si>
-    <t>East Bed Bath Shower - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Pantry - DIM TOGGLE</t>
-  </si>
-  <si>
-    <t>Wine Room - MOTION</t>
-  </si>
-  <si>
-    <t>Lower Hall - MOTION</t>
-  </si>
-  <si>
-    <t>Art Scene - UNKNOWN - Toggle</t>
-  </si>
-  <si>
-    <t>Bottom Floor Stairs - SWITCH ON</t>
-  </si>
-  <si>
-    <t>Pool Colored Lights - SWITCH TOGGLE</t>
-  </si>
-  <si>
-    <t>Jacuzzi Heater - TOGGLE LED FOR RTI</t>
-  </si>
-  <si>
-    <t>Jacuzzi Heater v2 - TOGGLE TASK LEDS</t>
-  </si>
-  <si>
-    <t>Whole House - GUEST SCENE</t>
-  </si>
-  <si>
-    <t>Whole House - OUTDOOR SCENE</t>
-  </si>
-  <si>
-    <t>Whole House - HOUSE OFF</t>
-  </si>
-  <si>
-    <t>Whole House - GOODBYE SCENE</t>
-  </si>
-  <si>
-    <t>Whole House - SLEEP SCENE</t>
-  </si>
-  <si>
-    <t>Whole House - MORNING SCENE</t>
-  </si>
-  <si>
-    <t>Whole House - BACKYARD SCENE TOGGLE</t>
-  </si>
-  <si>
-    <t>Jacuzzi Heater ON</t>
-  </si>
-  <si>
-    <t>Jacuzzi Heater OFF</t>
-  </si>
-  <si>
-    <t>Jacuzzi Heater v2 - TASK LED ON</t>
-  </si>
-  <si>
-    <t>Jacuzzi Heater v2 - TASK LED OFF</t>
-  </si>
-  <si>
-    <t>Volume + POOL ROOM</t>
-  </si>
-  <si>
-    <t>Volume - POOL ROOM</t>
-  </si>
-  <si>
-    <t>Gym - Exercise TOGGLE</t>
-  </si>
-  <si>
-    <t>Valence Lights ALL - Toggle</t>
-  </si>
-  <si>
-    <t>Volume + BILLIARDS AREA</t>
-  </si>
-  <si>
-    <t>Volume - BILLIARDS AREA</t>
-  </si>
-  <si>
-    <t>Volume + SUITE KITCHEN</t>
-  </si>
-  <si>
-    <t>Volume - SUITE KITCHEN</t>
-  </si>
-  <si>
-    <t>Volume + MAIN BED BATH</t>
-  </si>
-  <si>
-    <t>Volume - MAIN BED BATH</t>
-  </si>
-  <si>
-    <t>Volume + DINING ROOM</t>
-  </si>
-  <si>
-    <t>Page 4 of 5</t>
-  </si>
-  <si>
-    <t>Volume - DINING ROOM</t>
-  </si>
-  <si>
-    <t>Whole House -BRIGHT SCENE</t>
-  </si>
-  <si>
-    <t>Whole House -RELAX SCENE</t>
-  </si>
-  <si>
-    <t>Pool Camera Shut Off 3 hrs</t>
-  </si>
-  <si>
-    <t>East Bed Bath - OCC (Day/Night)</t>
-  </si>
-  <si>
-    <t>West Bed Bath - OCC (Day/Night)</t>
-  </si>
-  <si>
-    <t>Suite Bath - OCC (Day/Night)</t>
-  </si>
-  <si>
-    <t>Main Bed Bath - OCC (Day/Night)</t>
-  </si>
-  <si>
-    <t>Powder Room - OCC (Day/Night)</t>
-  </si>
-  <si>
-    <t>Billiards Area Bath - OCC (Day/Night)</t>
-  </si>
-  <si>
-    <t>East Bed Closet - OCC (Day/Night)</t>
-  </si>
-  <si>
-    <t>Main Bed Walk-In - OCC (Day/Night)</t>
-  </si>
-  <si>
-    <t>West Bed Closet - OCC (Day/Night)</t>
-  </si>
-  <si>
-    <t>Main Bed East Closet - OCC (Day/Night)</t>
-  </si>
-  <si>
-    <t>Suite Bed Closet - OCC (Day/Night)</t>
-  </si>
-  <si>
-    <t>Wine Room - OCC</t>
-  </si>
-  <si>
-    <t>Lower Hall - OCC</t>
-  </si>
-  <si>
-    <t>East and West Patio - SWITCH TOGGLE</t>
-  </si>
-  <si>
-    <t>Page 5 of 5</t>
   </si>
 </sst>
 </file>
@@ -1108,10 +1080,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1517,29 +1485,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -3355,7 +3300,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="11.13"/>
-    <col customWidth="1" min="2" max="2" width="9.63"/>
+    <col customWidth="1" min="2" max="2" width="17.88"/>
     <col customWidth="1" min="3" max="3" width="35.63"/>
   </cols>
   <sheetData>
@@ -4672,7 +4617,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="15.88"/>
+    <col customWidth="1" min="2" max="2" width="43.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4682,298 +4627,1373 @@
       <c r="B1" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>159</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="4">
-        <v>1.0</v>
+        <v>984.0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4">
-        <v>2.0</v>
+        <v>986.0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4">
-        <v>3.0</v>
+        <v>989.0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4">
-        <v>4.0</v>
+        <v>1000.0</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4">
-        <v>5.0</v>
+        <v>1001.0</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4">
-        <v>6.0</v>
+        <v>1004.0</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4">
-        <v>7.0</v>
+        <v>1006.0</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4">
-        <v>8.0</v>
+        <v>1008.0</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4">
-        <v>9.0</v>
+        <v>1009.0</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4">
-        <v>10.0</v>
+        <v>1010.0</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4">
-        <v>11.0</v>
+        <v>1013.0</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4">
-        <v>12.0</v>
+        <v>1014.0</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4">
-        <v>13.0</v>
+        <v>1021.0</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4">
-        <v>14.0</v>
+        <v>1024.0</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4">
-        <v>15.0</v>
+        <v>1035.0</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4">
-        <v>16.0</v>
+        <v>1054.0</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4">
-        <v>17.0</v>
+        <v>1062.0</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4">
-        <v>18.0</v>
+        <v>1119.0</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4">
-        <v>19.0</v>
+        <v>1158.0</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4">
-        <v>20.0</v>
+        <v>1198.0</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4">
-        <v>21.0</v>
+        <v>1199.0</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="4">
-        <v>22.0</v>
+        <v>1200.0</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4">
-        <v>23.0</v>
+        <v>1201.0</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4">
-        <v>24.0</v>
+        <v>1202.0</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4">
-        <v>25.0</v>
+        <v>1203.0</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4">
-        <v>26.0</v>
+        <v>1204.0</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4">
-        <v>27.0</v>
+        <v>1205.0</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="4">
-        <v>28.0</v>
+        <v>1206.0</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4">
-        <v>29.0</v>
+        <v>1207.0</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="4">
-        <v>30.0</v>
+        <v>1208.0</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4">
-        <v>31.0</v>
+        <v>1209.0</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="4">
-        <v>32.0</v>
+        <v>1210.0</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="4">
-        <v>33.0</v>
+        <v>1211.0</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="4">
-        <v>34.0</v>
+        <v>1213.0</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="4">
-        <v>35.0</v>
+        <v>1214.0</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="4">
-        <v>36.0</v>
+        <v>1215.0</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="4">
-        <v>37.0</v>
+        <v>1217.0</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="4">
-        <v>38.0</v>
+        <v>1219.0</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="4">
-        <v>39.0</v>
+        <v>1220.0</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="4">
-        <v>40.0</v>
+        <v>1222.0</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="4">
-        <v>41.0</v>
+        <v>1225.0</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="4">
-        <v>42.0</v>
+        <v>1231.0</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="4">
-        <v>43.0</v>
+        <v>1234.0</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="4">
-        <v>44.0</v>
+        <v>1235.0</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="4">
-        <v>45.0</v>
+        <v>1236.0</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="4">
-        <v>46.0</v>
+        <v>1238.0</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="4">
-        <v>47.0</v>
+        <v>1242.0</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="4">
-        <v>48.0</v>
+        <v>1243.0</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="4">
-        <v>49.0</v>
+        <v>1244.0</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="4">
-        <v>50.0</v>
+        <v>1247.0</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="4">
-        <v>51.0</v>
+        <v>1248.0</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="4">
-        <v>52.0</v>
+        <v>1249.0</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="4">
-        <v>53.0</v>
+        <v>1250.0</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="4">
-        <v>54.0</v>
+        <v>1251.0</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="4">
-        <v>55.0</v>
+        <v>1252.0</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="4">
-        <v>56.0</v>
+        <v>1258.0</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="4">
-        <v>57.0</v>
+        <v>1259.0</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="4">
-        <v>58.0</v>
+        <v>1260.0</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="4">
+        <v>1261.0</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="4">
+        <v>1262.0</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="4">
+        <v>1263.0</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="4">
+        <v>1265.0</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="4">
+        <v>1266.0</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="4">
+        <v>1267.0</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="4">
+        <v>1268.0</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="4">
+        <v>1269.0</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="4">
+        <v>1270.0</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="4">
+        <v>1271.0</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="4">
+        <v>1273.0</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="4">
+        <v>1274.0</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="4">
+        <v>1275.0</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="4">
+        <v>1276.0</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="4">
+        <v>1277.0</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="4">
+        <v>1278.0</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="4">
+        <v>1279.0</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="4">
+        <v>1280.0</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="4">
+        <v>1281.0</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="4">
+        <v>1282.0</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="4">
+        <v>1283.0</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="4">
+        <v>1284.0</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="4">
+        <v>1285.0</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="4">
+        <v>1286.0</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="4">
+        <v>1287.0</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="4">
+        <v>1288.0</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="4">
+        <v>1289.0</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="4">
+        <v>1291.0</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="4">
+        <v>1292.0</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="4">
+        <v>1293.0</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="4">
+        <v>1295.0</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="4">
+        <v>1297.0</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="4">
+        <v>1309.0</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="4">
+        <v>1310.0</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="4">
+        <v>1312.0</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="4">
+        <v>1313.0</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="4">
+        <v>1315.0</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="4">
+        <v>1316.0</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="4">
+        <v>1317.0</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="4">
+        <v>1318.0</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="4">
+        <v>1319.0</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="4">
+        <v>1320.0</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="4">
+        <v>1321.0</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="4">
+        <v>1322.0</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="4">
+        <v>1323.0</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="4">
+        <v>1324.0</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="4">
+        <v>1327.0</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="4">
+        <v>1328.0</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="4">
+        <v>1329.0</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="4">
+        <v>1330.0</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="4">
+        <v>1331.0</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="4">
+        <v>1332.0</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="4">
+        <v>1333.0</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="4">
+        <v>1334.0</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="4">
+        <v>1335.0</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="4">
+        <v>1336.0</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="4">
+        <v>1337.0</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="4">
+        <v>1338.0</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="4">
+        <v>1340.0</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="4">
+        <v>1341.0</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="4">
+        <v>1343.0</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="4">
+        <v>1344.0</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="4">
+        <v>1345.0</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="4">
+        <v>1352.0</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="4">
+        <v>1353.0</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="4">
+        <v>1354.0</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="4">
+        <v>1357.0</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="4">
+        <v>1360.0</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="4">
+        <v>1381.0</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="4">
+        <v>1386.0</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="4">
+        <v>1416.0</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="4">
+        <v>1417.0</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="4">
+        <v>1419.0</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="4">
+        <v>1421.0</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="4">
+        <v>1422.0</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="4">
+        <v>1423.0</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="4">
+        <v>1424.0</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="4">
+        <v>1425.0</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="4">
+        <v>1426.0</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="4">
+        <v>1429.0</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="4">
+        <v>1432.0</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="4">
+        <v>1433.0</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="4">
+        <v>1437.0</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="4">
+        <v>1438.0</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="4">
+        <v>1440.0</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="4">
+        <v>1441.0</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="4">
+        <v>1442.0</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="4">
+        <v>1443.0</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="4">
+        <v>1469.0</v>
+      </c>
+      <c r="B148" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="4">
+        <v>1471.0</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="4">
+        <v>1472.0</v>
+      </c>
+      <c r="B150" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="4">
+        <v>1473.0</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="4">
+        <v>1474.0</v>
+      </c>
+      <c r="B152" s="4" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="4">
+        <v>1475.0</v>
+      </c>
+      <c r="B153" s="4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="4">
+        <v>1476.0</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="4">
+        <v>1477.0</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="4">
+        <v>1478.0</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="4">
+        <v>1479.0</v>
+      </c>
+      <c r="B157" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="4">
+        <v>1480.0</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="4">
+        <v>1497.0</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="4">
+        <v>1500.0</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="4">
+        <v>1502.0</v>
+      </c>
+      <c r="B161" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="4">
+        <v>1504.0</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="4">
+        <v>1506.0</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="4">
+        <v>1507.0</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="4">
+        <v>1508.0</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="4">
+        <v>1509.0</v>
+      </c>
+      <c r="B166" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="4">
+        <v>1510.0</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="4">
+        <v>1511.0</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="4">
+        <v>1512.0</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="4">
+        <v>1515.0</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="4">
+        <v>1516.0</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="4">
+        <v>1518.0</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -4990,1444 +6010,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="2" max="2" width="43.75"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>160</v>
+        <v>330</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4">
-        <v>984.0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4">
-        <v>986.0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4">
-        <v>989.0</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4">
-        <v>1000.0</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4">
-        <v>1001.0</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4">
-        <v>1004.0</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4">
-        <v>1006.0</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4">
-        <v>1008.0</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4">
-        <v>1009.0</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="4">
-        <v>1010.0</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4">
-        <v>1013.0</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4">
-        <v>1014.0</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4">
-        <v>1021.0</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="4">
-        <v>1024.0</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4">
-        <v>1035.0</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="4">
-        <v>1054.0</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4">
-        <v>1062.0</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="4">
-        <v>1119.0</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4">
-        <v>1158.0</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="4">
-        <v>1198.0</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="4">
-        <v>1199.0</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="4">
-        <v>1200.0</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="4">
-        <v>1201.0</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="4">
-        <v>1202.0</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="4">
-        <v>1203.0</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="4">
-        <v>1204.0</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="4">
-        <v>1205.0</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="4">
-        <v>1206.0</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="4">
-        <v>1207.0</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="4">
-        <v>1208.0</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="4">
-        <v>1209.0</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="4">
-        <v>1210.0</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="4">
-        <v>1211.0</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="4">
-        <v>1213.0</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="4">
-        <v>1214.0</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="4">
-        <v>1215.0</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="4">
-        <v>1217.0</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="4">
-        <v>1219.0</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="4">
-        <v>1220.0</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="4">
-        <v>1222.0</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="4">
-        <v>1225.0</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="4">
-        <v>1231.0</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="4">
-        <v>1234.0</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="4">
-        <v>1235.0</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="4">
-        <v>1236.0</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="4">
-        <v>1238.0</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="4">
-        <v>1242.0</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="4">
-        <v>1243.0</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="4">
-        <v>1244.0</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="4">
-        <v>1247.0</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="4">
-        <v>1248.0</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="4">
-        <v>1249.0</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="4">
-        <v>1250.0</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="4">
-        <v>1251.0</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="4">
-        <v>1252.0</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="4">
-        <v>1258.0</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="4">
-        <v>1259.0</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="4">
-        <v>1260.0</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="4">
-        <v>1261.0</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="4">
-        <v>1262.0</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="4">
-        <v>1263.0</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="4">
-        <v>1265.0</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="4">
-        <v>1266.0</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="4">
-        <v>1267.0</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="4">
-        <v>1268.0</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="4">
-        <v>1269.0</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="4">
-        <v>1270.0</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="4">
-        <v>1271.0</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="4">
-        <v>1273.0</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="4">
-        <v>1274.0</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="4">
-        <v>1275.0</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="4">
-        <v>1276.0</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="4">
-        <v>1277.0</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="4">
-        <v>1278.0</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="4">
-        <v>1279.0</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="4" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="4">
-        <v>1280.0</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="4">
-        <v>1281.0</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="4">
-        <v>1282.0</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="4">
-        <v>1283.0</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="4">
-        <v>1284.0</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="4">
-        <v>1285.0</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="4">
-        <v>1286.0</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="4">
-        <v>1287.0</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="4">
-        <v>1288.0</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="4">
-        <v>1289.0</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="4">
-        <v>1291.0</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="4">
-        <v>1292.0</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="4">
-        <v>1293.0</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="4">
-        <v>1295.0</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="4">
-        <v>1297.0</v>
-      </c>
-      <c r="B98" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="4">
-        <v>1309.0</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="4">
-        <v>1310.0</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="4">
-        <v>1312.0</v>
-      </c>
-      <c r="B101" s="4" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="4">
-        <v>1313.0</v>
-      </c>
-      <c r="B102" s="4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="4">
-        <v>1315.0</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="4">
-        <v>1316.0</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="4">
-        <v>1317.0</v>
-      </c>
-      <c r="B105" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="4">
-        <v>1318.0</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="4">
-        <v>1319.0</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="4">
-        <v>1320.0</v>
-      </c>
-      <c r="B108" s="4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="4">
-        <v>1321.0</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="4">
-        <v>1322.0</v>
-      </c>
-      <c r="B110" s="4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="4">
-        <v>1323.0</v>
-      </c>
-      <c r="B111" s="4" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="4">
-        <v>1324.0</v>
-      </c>
-      <c r="B112" s="4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="4">
-        <v>1327.0</v>
-      </c>
-      <c r="B113" s="4" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="4">
-        <v>1328.0</v>
-      </c>
-      <c r="B114" s="4" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="4">
-        <v>1329.0</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="4">
-        <v>1330.0</v>
-      </c>
-      <c r="B116" s="4" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="4">
-        <v>1331.0</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="4">
-        <v>1332.0</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="4">
-        <v>1333.0</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="4">
-        <v>1334.0</v>
-      </c>
-      <c r="B120" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B121" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="C121" s="4" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="4">
-        <v>1335.0</v>
-      </c>
-      <c r="B124" s="4" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" s="4">
-        <v>1336.0</v>
-      </c>
-      <c r="B125" s="4" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="4">
-        <v>1337.0</v>
-      </c>
-      <c r="B126" s="4" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" s="4">
-        <v>1338.0</v>
-      </c>
-      <c r="B127" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" s="4">
-        <v>1340.0</v>
-      </c>
-      <c r="B128" s="4" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" s="4">
-        <v>1341.0</v>
-      </c>
-      <c r="B129" s="4" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="4">
-        <v>1343.0</v>
-      </c>
-      <c r="B130" s="4" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" s="4">
-        <v>1344.0</v>
-      </c>
-      <c r="B131" s="4" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="4">
-        <v>1345.0</v>
-      </c>
-      <c r="B132" s="4" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" s="4">
-        <v>1352.0</v>
-      </c>
-      <c r="B133" s="4" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" s="4">
-        <v>1353.0</v>
-      </c>
-      <c r="B134" s="4" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" s="4">
-        <v>1354.0</v>
-      </c>
-      <c r="B135" s="4" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" s="4">
-        <v>1357.0</v>
-      </c>
-      <c r="B136" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" s="4">
-        <v>1360.0</v>
-      </c>
-      <c r="B137" s="4" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" s="4">
-        <v>1381.0</v>
-      </c>
-      <c r="B138" s="4" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" s="4">
-        <v>1386.0</v>
-      </c>
-      <c r="B139" s="4" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" s="4">
-        <v>1416.0</v>
-      </c>
-      <c r="B140" s="4" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" s="4">
-        <v>1417.0</v>
-      </c>
-      <c r="B141" s="4" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" s="4">
-        <v>1419.0</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" s="4">
-        <v>1421.0</v>
-      </c>
-      <c r="B143" s="4" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" s="4">
-        <v>1422.0</v>
-      </c>
-      <c r="B144" s="4" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" s="4">
-        <v>1423.0</v>
-      </c>
-      <c r="B145" s="4" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" s="4">
-        <v>1424.0</v>
-      </c>
-      <c r="B146" s="4" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" s="4">
-        <v>1425.0</v>
-      </c>
-      <c r="B147" s="4" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" s="4">
-        <v>1426.0</v>
-      </c>
-      <c r="B148" s="4" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" s="4">
-        <v>1429.0</v>
-      </c>
-      <c r="B149" s="4" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" s="4">
-        <v>1432.0</v>
-      </c>
-      <c r="B150" s="4" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" s="4">
-        <v>1433.0</v>
-      </c>
-      <c r="B151" s="4" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" s="4">
-        <v>1437.0</v>
-      </c>
-      <c r="B152" s="4" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" s="4">
-        <v>1438.0</v>
-      </c>
-      <c r="B153" s="4" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" s="4">
-        <v>1440.0</v>
-      </c>
-      <c r="B154" s="4" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" s="4">
-        <v>1441.0</v>
-      </c>
-      <c r="B155" s="4" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" s="4">
-        <v>1442.0</v>
-      </c>
-      <c r="B156" s="4" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" s="4">
-        <v>1443.0</v>
-      </c>
-      <c r="B157" s="4" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" s="4">
-        <v>1469.0</v>
-      </c>
-      <c r="B158" s="4" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" s="4">
-        <v>1471.0</v>
-      </c>
-      <c r="B159" s="4" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" s="4">
-        <v>1472.0</v>
-      </c>
-      <c r="B160" s="4" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" s="4">
-        <v>1473.0</v>
-      </c>
-      <c r="B161" s="4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" s="4">
-        <v>1474.0</v>
-      </c>
-      <c r="B162" s="4" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" s="4">
-        <v>1475.0</v>
-      </c>
-      <c r="B163" s="4" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" s="4">
-        <v>1476.0</v>
-      </c>
-      <c r="B164" s="4" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B165" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="C165" s="4" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" s="4">
-        <v>1477.0</v>
-      </c>
-      <c r="B168" s="4" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" s="4">
-        <v>1478.0</v>
-      </c>
-      <c r="B169" s="4" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" s="4">
-        <v>1479.0</v>
-      </c>
-      <c r="B170" s="4" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" s="4">
-        <v>1480.0</v>
-      </c>
-      <c r="B171" s="4" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" s="4">
-        <v>1497.0</v>
-      </c>
-      <c r="B172" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" s="4">
-        <v>1500.0</v>
-      </c>
-      <c r="B173" s="4" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" s="4">
-        <v>1502.0</v>
-      </c>
-      <c r="B174" s="4" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" s="4">
-        <v>1504.0</v>
-      </c>
-      <c r="B175" s="4" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" s="4">
-        <v>1506.0</v>
-      </c>
-      <c r="B176" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" s="4">
-        <v>1507.0</v>
-      </c>
-      <c r="B177" s="4" t="s">
         <v>331</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" s="4">
-        <v>1508.0</v>
-      </c>
-      <c r="B178" s="4" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" s="4">
-        <v>1509.0</v>
-      </c>
-      <c r="B179" s="4" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" s="4">
-        <v>1510.0</v>
-      </c>
-      <c r="B180" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" s="4">
-        <v>1511.0</v>
-      </c>
-      <c r="B181" s="4" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" s="4">
-        <v>1512.0</v>
-      </c>
-      <c r="B182" s="4" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="4">
-        <v>1515.0</v>
-      </c>
-      <c r="B183" s="4" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" s="4">
-        <v>1516.0</v>
-      </c>
-      <c r="B184" s="4" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" s="4">
-        <v>1518.0</v>
-      </c>
-      <c r="B185" s="4" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B186" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="C186" s="4" t="s">
-        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>